<commit_message>
Tax scales back to 1989-90
</commit_message>
<xml_diff>
--- a/data-raw/tax_brackets_and_marginal_rates.xlsx
+++ b/data-raw/tax_brackets_and_marginal_rates.xlsx
@@ -1,32 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hugh\Documents\GitHub\grattan\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hugh Parsonage\Documents\Github\grattan\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="9" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="2003-04" sheetId="4" r:id="rId2"/>
-    <sheet name="2004-05" sheetId="5" r:id="rId3"/>
-    <sheet name="2005-06" sheetId="6" r:id="rId4"/>
-    <sheet name="2006-07" sheetId="7" r:id="rId5"/>
-    <sheet name="2007-08" sheetId="8" r:id="rId6"/>
-    <sheet name="2008-09" sheetId="9" r:id="rId7"/>
-    <sheet name="2009-10" sheetId="10" r:id="rId8"/>
-    <sheet name="2010-11" sheetId="11" r:id="rId9"/>
-    <sheet name="2011-12" sheetId="12" r:id="rId10"/>
-    <sheet name="2012-13" sheetId="2" r:id="rId11"/>
-    <sheet name="2013-14" sheetId="3" r:id="rId12"/>
-    <sheet name="2014-15" sheetId="13" r:id="rId13"/>
-    <sheet name="2015-16" sheetId="14" r:id="rId14"/>
-    <sheet name="2016-17" sheetId="15" r:id="rId15"/>
+    <sheet name="1989-90" sheetId="29" r:id="rId2"/>
+    <sheet name="1990-91" sheetId="28" r:id="rId3"/>
+    <sheet name="1991-92" sheetId="27" r:id="rId4"/>
+    <sheet name="1992-93" sheetId="26" r:id="rId5"/>
+    <sheet name="1993-94" sheetId="25" r:id="rId6"/>
+    <sheet name="1994-95" sheetId="24" r:id="rId7"/>
+    <sheet name="1995-96" sheetId="23" r:id="rId8"/>
+    <sheet name="1996-97" sheetId="22" r:id="rId9"/>
+    <sheet name="1997-98" sheetId="21" r:id="rId10"/>
+    <sheet name="1998-99" sheetId="20" r:id="rId11"/>
+    <sheet name="1999-00" sheetId="19" r:id="rId12"/>
+    <sheet name="2000-01" sheetId="18" r:id="rId13"/>
+    <sheet name="2001-02" sheetId="17" r:id="rId14"/>
+    <sheet name="2002-03" sheetId="16" r:id="rId15"/>
+    <sheet name="2003-04" sheetId="4" r:id="rId16"/>
+    <sheet name="2004-05" sheetId="5" r:id="rId17"/>
+    <sheet name="2005-06" sheetId="6" r:id="rId18"/>
+    <sheet name="2006-07" sheetId="7" r:id="rId19"/>
+    <sheet name="2007-08" sheetId="8" r:id="rId20"/>
+    <sheet name="2008-09" sheetId="9" r:id="rId21"/>
+    <sheet name="2009-10" sheetId="10" r:id="rId22"/>
+    <sheet name="2010-11" sheetId="11" r:id="rId23"/>
+    <sheet name="2011-12" sheetId="12" r:id="rId24"/>
+    <sheet name="2012-13" sheetId="2" r:id="rId25"/>
+    <sheet name="2013-14" sheetId="3" r:id="rId26"/>
+    <sheet name="2014-15" sheetId="13" r:id="rId27"/>
+    <sheet name="2015-16" sheetId="14" r:id="rId28"/>
+    <sheet name="2016-17" sheetId="15" r:id="rId29"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -38,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="2">
   <si>
     <t>lower_brackets</t>
   </si>
@@ -49,7 +63,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -174,6 +188,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -209,6 +240,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -376,6 +424,959 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5400</v>
+      </c>
+      <c r="B3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>20700</v>
+      </c>
+      <c r="B4">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>38000</v>
+      </c>
+      <c r="B5">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>50000</v>
+      </c>
+      <c r="B6">
+        <v>0.47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5400</v>
+      </c>
+      <c r="B3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>20700</v>
+      </c>
+      <c r="B4">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>38000</v>
+      </c>
+      <c r="B5">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>50000</v>
+      </c>
+      <c r="B6">
+        <v>0.47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5400</v>
+      </c>
+      <c r="B3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>20700</v>
+      </c>
+      <c r="B4">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>38000</v>
+      </c>
+      <c r="B5">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>50000</v>
+      </c>
+      <c r="B6">
+        <v>0.47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>6000</v>
+      </c>
+      <c r="B3">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>20000</v>
+      </c>
+      <c r="B4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>50000</v>
+      </c>
+      <c r="B5">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>60000</v>
+      </c>
+      <c r="B6">
+        <v>0.47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>6000</v>
+      </c>
+      <c r="B3">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>20000</v>
+      </c>
+      <c r="B4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>50000</v>
+      </c>
+      <c r="B5">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>60000</v>
+      </c>
+      <c r="B6">
+        <v>0.47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>6000</v>
+      </c>
+      <c r="B3">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>20000</v>
+      </c>
+      <c r="B4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>50000</v>
+      </c>
+      <c r="B5">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>60000</v>
+      </c>
+      <c r="B6">
+        <v>0.47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>6000</v>
+      </c>
+      <c r="B3">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>21600</v>
+      </c>
+      <c r="B4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>52000</v>
+      </c>
+      <c r="B5">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>62500</v>
+      </c>
+      <c r="B6">
+        <v>0.47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>6000</v>
+      </c>
+      <c r="B3">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>21600</v>
+      </c>
+      <c r="B4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>58000</v>
+      </c>
+      <c r="B5">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>70000</v>
+      </c>
+      <c r="B6">
+        <v>0.47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>6000</v>
+      </c>
+      <c r="B3">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>21600</v>
+      </c>
+      <c r="B4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>63000</v>
+      </c>
+      <c r="B5">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>95000</v>
+      </c>
+      <c r="B6">
+        <v>0.47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>6000</v>
+      </c>
+      <c r="B3">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>25000</v>
+      </c>
+      <c r="B4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>75000</v>
+      </c>
+      <c r="B5">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>150000</v>
+      </c>
+      <c r="B6">
+        <v>0.45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5100</v>
+      </c>
+      <c r="B3">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>17650</v>
+      </c>
+      <c r="B4">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>20600</v>
+      </c>
+      <c r="B5">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>35000</v>
+      </c>
+      <c r="B6">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>50000</v>
+      </c>
+      <c r="B7">
+        <v>0.48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>6000</v>
+      </c>
+      <c r="B3">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>30000</v>
+      </c>
+      <c r="B4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>75000</v>
+      </c>
+      <c r="B5">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>150000</v>
+      </c>
+      <c r="B6">
+        <v>0.45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>6000</v>
+      </c>
+      <c r="B3">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>34000</v>
+      </c>
+      <c r="B4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>80000</v>
+      </c>
+      <c r="B5">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>180000</v>
+      </c>
+      <c r="B6">
+        <v>0.45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>6000</v>
+      </c>
+      <c r="B3">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>35000</v>
+      </c>
+      <c r="B4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>80000</v>
+      </c>
+      <c r="B5">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>180000</v>
+      </c>
+      <c r="B6">
+        <v>0.45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>6000</v>
+      </c>
+      <c r="B3">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>35000</v>
+      </c>
+      <c r="B4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>80000</v>
+      </c>
+      <c r="B5">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>180000</v>
+      </c>
+      <c r="B6">
+        <v>0.45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -434,7 +1435,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -500,7 +1501,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -563,7 +1564,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -626,7 +1627,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -689,11 +1690,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -752,7 +1753,94 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5250</v>
+      </c>
+      <c r="B3">
+        <v>0.20499999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>17650</v>
+      </c>
+      <c r="B4">
+        <v>0.245</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>20600</v>
+      </c>
+      <c r="B5">
+        <v>0.29499999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>20700</v>
+      </c>
+      <c r="B6">
+        <v>0.38500000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>35000</v>
+      </c>
+      <c r="B7">
+        <v>0.42499999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>36000</v>
+      </c>
+      <c r="B8">
+        <v>0.46500000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>50000</v>
+      </c>
+      <c r="B9">
+        <v>0.47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -780,31 +1868,31 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>6000</v>
-      </c>
-      <c r="B3">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>21600</v>
-      </c>
-      <c r="B4">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>52000</v>
-      </c>
-      <c r="B5">
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>62500</v>
+        <v>5400</v>
+      </c>
+      <c r="B3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>20700</v>
+      </c>
+      <c r="B4">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>36000</v>
+      </c>
+      <c r="B5">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>50000</v>
       </c>
       <c r="B6">
         <v>0.47</v>
@@ -815,9 +1903,72 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5400</v>
+      </c>
+      <c r="B3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>20700</v>
+      </c>
+      <c r="B4">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>36000</v>
+      </c>
+      <c r="B5">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>50000</v>
+      </c>
+      <c r="B6">
+        <v>0.47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -843,33 +1994,41 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>6000</v>
-      </c>
-      <c r="B3">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>21600</v>
-      </c>
-      <c r="B4">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>58000</v>
-      </c>
-      <c r="B5">
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>70000</v>
-      </c>
-      <c r="B6">
+        <v>5400</v>
+      </c>
+      <c r="B3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>20700</v>
+      </c>
+      <c r="B4">
+        <v>0.35499999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>36000</v>
+      </c>
+      <c r="B5">
+        <v>0.38500000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>38000</v>
+      </c>
+      <c r="B6">
+        <v>0.44124999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>50000</v>
+      </c>
+      <c r="B7">
         <v>0.47</v>
       </c>
     </row>
@@ -878,7 +2037,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -906,31 +2065,31 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>6000</v>
-      </c>
-      <c r="B3">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>21600</v>
-      </c>
-      <c r="B4">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>63000</v>
-      </c>
-      <c r="B5">
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>95000</v>
+        <v>5400</v>
+      </c>
+      <c r="B3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>20700</v>
+      </c>
+      <c r="B4">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>38000</v>
+      </c>
+      <c r="B5">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>50000</v>
       </c>
       <c r="B6">
         <v>0.47</v>
@@ -941,7 +2100,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -969,42 +2128,42 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>6000</v>
-      </c>
-      <c r="B3">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>25000</v>
-      </c>
-      <c r="B4">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>75000</v>
-      </c>
-      <c r="B5">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>150000</v>
-      </c>
-      <c r="B6">
-        <v>0.45</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>5400</v>
+      </c>
+      <c r="B3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>20700</v>
+      </c>
+      <c r="B4">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>38000</v>
+      </c>
+      <c r="B5">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>50000</v>
+      </c>
+      <c r="B6">
+        <v>0.47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1032,223 +2191,34 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>6000</v>
-      </c>
-      <c r="B3">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>30000</v>
-      </c>
-      <c r="B4">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>75000</v>
-      </c>
-      <c r="B5">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>150000</v>
-      </c>
-      <c r="B6">
-        <v>0.45</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>6000</v>
-      </c>
-      <c r="B3">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>34000</v>
-      </c>
-      <c r="B4">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>80000</v>
-      </c>
-      <c r="B5">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>180000</v>
-      </c>
-      <c r="B6">
-        <v>0.45</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>6000</v>
-      </c>
-      <c r="B3">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>35000</v>
-      </c>
-      <c r="B4">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>80000</v>
-      </c>
-      <c r="B5">
-        <v>0.38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>180000</v>
-      </c>
-      <c r="B6">
-        <v>0.45</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>6000</v>
-      </c>
-      <c r="B3">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>35000</v>
-      </c>
-      <c r="B4">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>80000</v>
-      </c>
-      <c r="B5">
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>180000</v>
-      </c>
-      <c r="B6">
-        <v>0.45</v>
+        <v>5400</v>
+      </c>
+      <c r="B3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>20700</v>
+      </c>
+      <c r="B4">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>38000</v>
+      </c>
+      <c r="B5">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>50000</v>
+      </c>
+      <c r="B6">
+        <v>0.47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>